<commit_message>
Changed 6p connector id
</commit_message>
<xml_diff>
--- a/cam/RP2040-Eins-20231104-JLCPCB-BOM-SOIC.xlsx
+++ b/cam/RP2040-Eins-20231104-JLCPCB-BOM-SOIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E2D541-BDCE-49E0-B6F3-9CFA6FF7E7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D77172-B345-4FD9-9C4B-3E3237E00E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23004" yWindow="1548" windowWidth="11004" windowHeight="21360" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
+    <workbookView xWindow="2868" yWindow="1680" windowWidth="14148" windowHeight="21360" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,9 +370,6 @@
     <t>C16214</t>
   </si>
   <si>
-    <t>C2935977</t>
-  </si>
-  <si>
     <t>Plugin,P=2.54mm</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>Q4,Q3,Q5,Q2</t>
+  </si>
+  <si>
+    <t>C40877</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,10 +914,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -1101,10 +1101,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
         <v>108</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1115,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>82</v>
@@ -1135,10 +1135,10 @@
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" t="s">
         <v>39</v>
@@ -1152,10 +1152,10 @@
         <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
         <v>41</v>
@@ -1271,10 +1271,10 @@
         <v>54</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
         <v>108</v>
-      </c>
-      <c r="D30" t="s">
-        <v>109</v>
       </c>
       <c r="E30" t="s">
         <v>55</v>
@@ -1291,7 +1291,7 @@
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
         <v>57</v>
@@ -1305,10 +1305,10 @@
         <v>58</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
         <v>59</v>

</xml_diff>